<commit_message>
Bookmarks data extracted. pdf_testcases has been edited to reflect the bookmarks property
git-svn-id: http://pdfainspector.googlecode.com/svn/trunk@96 1783f179-91b5-6867-892f-c6e3ac0b0089
</commit_message>
<xml_diff>
--- a/testcases/charts/pdf_testcases.xlsx
+++ b/testcases/charts/pdf_testcases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="7395" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="7395"/>
   </bookViews>
   <sheets>
     <sheet name="All test cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="108">
   <si>
     <t>Filename</t>
   </si>
@@ -54,9 +54,6 @@
     <t>tables-tagged</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>text and table, no tags</t>
   </si>
   <si>
@@ -103,12 +100,6 @@
   </si>
   <si>
     <t>directly converted from Word</t>
-  </si>
-  <si>
-    <t>generated by me (using itext)</t>
-  </si>
-  <si>
-    <t>text only, colored text</t>
   </si>
   <si>
     <t>text only, bold/formatting</t>
@@ -354,6 +345,9 @@
   <si>
     <t>&lt;Table Alt="Table of Names and Colors"&gt;
 No &lt;span&gt; tags</t>
+  </si>
+  <si>
+    <t>Bookmarks</t>
   </si>
 </sst>
 </file>
@@ -727,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G24:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -740,883 +734,898 @@
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="33.28515625" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
+      <c r="G2" s="2"/>
       <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>36</v>
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>53</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>54</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="4">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>55</v>
+        <v>25</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>54</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>55</v>
+        <v>16</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>54</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>36</v>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="4">
+        <v>16</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="4">
         <v>2</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="K8" s="3" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>55</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
+      <c r="G9" s="2"/>
       <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="2">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="2">
         <v>6</v>
       </c>
-      <c r="J9" t="s">
-        <v>36</v>
-      </c>
       <c r="K9" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="L9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="M9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="G10" s="2"/>
       <c r="H10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>37</v>
+        <v>74</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>34</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
+      <c r="G11" s="2"/>
       <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="L11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="M11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>22</v>
+        <v>66</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="4">
+        <v>21</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="4">
         <v>3</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="3" t="s">
-        <v>31</v>
+      <c r="G13" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="4">
+        <v>28</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="4">
         <v>3</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="K13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>33</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="G14" s="4"/>
       <c r="H14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="4">
-        <v>1</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>105</v>
+        <v>51</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>104</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="6">
-        <v>1</v>
-      </c>
-      <c r="J15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K15" t="s">
-        <v>64</v>
-      </c>
-      <c r="L15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="4">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="B17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="G17" s="6"/>
       <c r="H17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="6">
-        <v>1</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" t="s">
-        <v>64</v>
+        <v>16</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="6">
+        <v>1</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="L17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="M17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="G18" s="4"/>
       <c r="H18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="4">
-        <v>1</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>91</v>
+        <v>51</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1</v>
       </c>
       <c r="K18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" t="s">
-        <v>17</v>
-      </c>
+      <c r="G19" s="2"/>
       <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="2">
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="2">
         <v>3</v>
       </c>
-      <c r="J19" t="s">
-        <v>36</v>
-      </c>
       <c r="K19" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="L19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="M19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="G20" s="4"/>
       <c r="H20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>103</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="3" t="s">
-        <v>26</v>
+      <c r="G21" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="4">
-        <v>1</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="3" t="s">
-        <v>26</v>
+      <c r="G22" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="4">
-        <v>1</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="4">
+        <v>1</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>33</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" t="s">
-        <v>26</v>
-      </c>
+      <c r="G23" s="2"/>
       <c r="H23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="2">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="L23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="M23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>22</v>
+        <v>66</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="4">
-        <v>1</v>
-      </c>
-      <c r="J24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="4">
+        <v>1</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" t="s">
         <v>60</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F25" s="4"/>
-      <c r="G25" s="3" t="s">
-        <v>20</v>
+      <c r="G25" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="4">
-        <v>1</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="C26" s="4"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="2">
-        <v>1</v>
-      </c>
-      <c r="J26" t="s">
-        <v>36</v>
-      </c>
-      <c r="K26" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="G26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1627,400 +1636,428 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="10" max="10" width="37.140625" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>59</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="8">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>55</v>
+        <v>66</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8">
+        <v>1</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>52</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="8">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>55</v>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="8">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>55</v>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8">
+        <v>1</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>52</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="8">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>55</v>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8">
+        <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="45">
+        <v>52</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="8">
+        <v>66</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="8">
         <v>3</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>76</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8">
+      <c r="G7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="8">
         <v>3</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="I7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>33</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>102</v>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8">
+        <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10">
+        <v>99</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>103</v>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8">
+        <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="35.25" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="J9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="B10" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="8">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>108</v>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8">
+        <v>1</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>105</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="8">
-        <v>1</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>36</v>
+      <c r="G11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>33</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="8">
-        <v>1</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>36</v>
+      <c r="G12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="J12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30">
+        <v>33</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>82</v>
+        <v>66</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>79</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F14" s="8"/>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>36</v>
+      <c r="G14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="J14" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "Standard Tags" column for test cases
git-svn-id: http://pdfainspector.googlecode.com/svn/trunk@100 1783f179-91b5-6867-892f-c6e3ac0b0089
</commit_message>
<xml_diff>
--- a/testcases/charts/pdf_testcases.xlsx
+++ b/testcases/charts/pdf_testcases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="117">
   <si>
     <t>Filename</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Additional Comments</t>
   </si>
   <si>
-    <t>directly converted from Word</t>
-  </si>
-  <si>
     <t>text only, bold/formatting</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>blank xml file</t>
   </si>
   <si>
-    <t>tagged text</t>
-  </si>
-  <si>
     <t>Features</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>starbucks_textonly-primopdf</t>
   </si>
   <si>
-    <t>generated by primopdf plugin through MSWord</t>
-  </si>
-  <si>
     <t>&lt;sect&gt;, &lt;p&gt;</t>
   </si>
   <si>
@@ -177,13 +168,7 @@
     <t>blank &lt;Document&gt; &lt;/Document&gt; xml file</t>
   </si>
   <si>
-    <t>generated by MSWord's "save as PDF"</t>
-  </si>
-  <si>
     <t>(fuller xml than itext. See file for more details.)</t>
-  </si>
-  <si>
-    <t>Same*</t>
   </si>
   <si>
     <t>headings contain id names, otherwise same*</t>
@@ -288,12 +273,6 @@
     <t>starbucks_untaggedimageonly-msword</t>
   </si>
   <si>
-    <t>tagged xml file</t>
-  </si>
-  <si>
-    <t>* = all Adobe Acrobat xml outputs have information about the xml/pdf file (metadata) that itext does not create.</t>
-  </si>
-  <si>
     <t>autofills for image tag w/ filename of image</t>
   </si>
   <si>
@@ -303,12 +282,6 @@
     <t>&lt;Figure Alt="starbucks.jpg"&gt; (autofills for image tag w/ filename of image)</t>
   </si>
   <si>
-    <t>generated by MSWord's "save as PDF"; untagged image</t>
-  </si>
-  <si>
-    <t>generated by MSWord's "save as PDF"; image tagged via Acrobat Pro</t>
-  </si>
-  <si>
     <t>tables-example2</t>
   </si>
   <si>
@@ -316,9 +289,6 @@
   </si>
   <si>
     <t>table only</t>
-  </si>
-  <si>
-    <t>generated by MSWord's "save as PDF"; tagged later with Acrobat Pro</t>
   </si>
   <si>
     <t>&lt;figure&gt;&lt;/figure&gt;</t>
@@ -348,6 +318,63 @@
   </si>
   <si>
     <t>Bookmarks</t>
+  </si>
+  <si>
+    <t>Standard Tags</t>
+  </si>
+  <si>
+    <t>header, normal</t>
+  </si>
+  <si>
+    <t>&lt;sect&gt;, &lt;normal&gt;, &lt;heading&gt;, etc.</t>
+  </si>
+  <si>
+    <t>header, normal, (form tags)</t>
+  </si>
+  <si>
+    <t>Same as itext (w/ metadata)</t>
+  </si>
+  <si>
+    <t>image is untagged</t>
+  </si>
+  <si>
+    <t>image tagged</t>
+  </si>
+  <si>
+    <t>Generator</t>
+  </si>
+  <si>
+    <t>InDesign CS3</t>
+  </si>
+  <si>
+    <t>InDesign CS4</t>
+  </si>
+  <si>
+    <t>InDesign CS5</t>
+  </si>
+  <si>
+    <t>InDesign CS6</t>
+  </si>
+  <si>
+    <t>MSWord's "save as PDF"; image tagged via Acrobat Pro</t>
+  </si>
+  <si>
+    <t>primopdf plugin through MSWord</t>
+  </si>
+  <si>
+    <t>MSWord's "save as PDF"</t>
+  </si>
+  <si>
+    <t>MSWord's "save as PDF"; tagged later with Acrobat Pro</t>
+  </si>
+  <si>
+    <t>MSWord</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MSWord &amp; Adobe Acrobat</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -721,29 +748,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G24:G25"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="33.28515625" customWidth="1"/>
-    <col min="13" max="13" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,248 +779,265 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>54</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>33</v>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="4">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>52</v>
+      <c r="J5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>50</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4"/>
+      <c r="I6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>52</v>
+      <c r="J6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>50</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1000,99 +1045,109 @@
         <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4">
         <v>2</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>55</v>
+      <c r="L8" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>102</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>66</v>
+      <c r="C9" s="2"/>
+      <c r="D9" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="G9" s="2"/>
-      <c r="H9" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" t="s">
         <v>18</v>
       </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2">
         <v>6</v>
       </c>
-      <c r="K9" t="s">
-        <v>33</v>
-      </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>69</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1100,71 +1155,77 @@
         <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="G11" s="2"/>
-      <c r="H11" t="s">
+      <c r="H11" s="2"/>
+      <c r="I11" t="s">
         <v>19</v>
       </c>
-      <c r="I11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="2">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>33</v>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="4">
         <v>3</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="L12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>52</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -1172,461 +1233,489 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>28</v>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="4">
+        <v>27</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="4">
         <v>3</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="L13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>32</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="H14" s="4"/>
       <c r="I14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="4">
-        <v>1</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="5" t="s">
-        <v>51</v>
-      </c>
+      <c r="H15" s="6"/>
       <c r="I15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="6">
-        <v>1</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="6">
+        <v>1</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="M15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="4"/>
+      <c r="I16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="4">
-        <v>1</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>55</v>
+      <c r="J16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>102</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="6">
-        <v>1</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" t="s">
-        <v>61</v>
+      <c r="J17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="6">
+        <v>1</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="M17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="H18" s="4"/>
       <c r="I18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="4">
-        <v>1</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>90</v>
+        <v>103</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>83</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" t="s">
+      <c r="H19" s="2"/>
+      <c r="I19" t="s">
         <v>16</v>
       </c>
-      <c r="I19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="2">
+      <c r="J19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="2">
         <v>3</v>
       </c>
-      <c r="K19" t="s">
-        <v>33</v>
-      </c>
       <c r="L19" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="H20" s="4"/>
       <c r="I20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="4">
-        <v>1</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+        <v>93</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="4">
-        <v>1</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>33</v>
+      <c r="J21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="3" t="s">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" s="4">
-        <v>1</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>33</v>
+      <c r="J22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="4">
+        <v>1</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>32</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" t="s">
+      <c r="H23" s="2"/>
+      <c r="I23" t="s">
         <v>25</v>
       </c>
-      <c r="I23" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="2">
-        <v>1</v>
-      </c>
-      <c r="K23" t="s">
-        <v>33</v>
+      <c r="J23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="4">
-        <v>1</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L24" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="4">
-        <v>1</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="C26" s="4"/>
-      <c r="D26" s="2"/>
+      <c r="N25" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="D26" s="4"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" t="s">
-        <v>89</v>
-      </c>
+      <c r="H26" s="2"/>
+      <c r="K26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1659,19 +1748,19 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
@@ -1680,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>26</v>
@@ -1688,44 +1777,44 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8">
         <v>1</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -1733,27 +1822,27 @@
         <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -1762,24 +1851,24 @@
         <v>1</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1789,13 +1878,13 @@
         <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45">
@@ -1806,27 +1895,27 @@
         <v>20</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H6" s="8">
         <v>3</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1834,41 +1923,41 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H7" s="8">
         <v>3</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -1876,24 +1965,24 @@
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1901,27 +1990,27 @@
         <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="35.25" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -1930,10 +2019,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1941,30 +2030,30 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H11" s="8">
         <v>1</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1972,92 +2061,92 @@
         <v>5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H12" s="8">
         <v>1</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H13" s="8">
         <v>1</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H14" s="8">
         <v>1</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional test cases created for the bookmark/header rules.
git-svn-id: http://pdfainspector.googlecode.com/svn/trunk@189 1783f179-91b5-6867-892f-c6e3ac0b0089
</commit_message>
<xml_diff>
--- a/testcases/charts/pdf_testcases.xlsx
+++ b/testcases/charts/pdf_testcases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="121">
   <si>
     <t>Filename</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t>&lt;sect&gt;, &lt;h1&gt;, &lt;p&gt;</t>
+  </si>
+  <si>
+    <t>eight_pages</t>
+  </si>
+  <si>
+    <t>text and bookmarks</t>
+  </si>
+  <si>
+    <t>&lt;sect&gt;,&lt;h1&gt;,&lt;h2&gt;,&lt;p&gt;</t>
   </si>
 </sst>
 </file>
@@ -751,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -855,92 +864,86 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="4">
-        <v>13</v>
-      </c>
-      <c r="L3" s="3"/>
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2">
+        <v>8</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="3" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>115</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>14</v>
@@ -955,30 +958,30 @@
         <v>50</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>115</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="3" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>14</v>
@@ -993,12 +996,12 @@
         <v>50</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>45</v>
@@ -1009,12 +1012,14 @@
       <c r="D7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>14</v>
@@ -1029,254 +1034,252 @@
         <v>50</v>
       </c>
       <c r="N7" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" t="s">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" t="s">
         <v>15</v>
       </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
         <v>32</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" t="s">
         <v>55</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:14">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3" t="s">
+      <c r="D10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="4">
+      <c r="J10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="4">
         <v>2</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M9" s="3" t="s">
+      <c r="L10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="2">
-        <v>6</v>
-      </c>
-      <c r="L10" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" t="s">
-        <v>55</v>
-      </c>
-      <c r="N10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
         <v>14</v>
       </c>
       <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>113</v>
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
+      <c r="A12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" t="s">
+      <c r="I12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" t="s">
         <v>19</v>
       </c>
-      <c r="J12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
         <v>32</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M13" t="s">
         <v>55</v>
       </c>
-      <c r="N12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="4">
-        <v>3</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="N13" s="3" t="s">
+      <c r="N13" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H14" s="4" t="s">
         <v>60</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>14</v>
@@ -1284,11 +1287,11 @@
       <c r="K14" s="4">
         <v>3</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>32</v>
+      <c r="L14" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>113</v>
@@ -1296,275 +1299,273 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="4">
+        <v>3</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="3" t="s">
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="4">
-        <v>1</v>
-      </c>
-      <c r="L15" s="3" t="s">
+      <c r="J16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:14">
+      <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="6">
-        <v>1</v>
-      </c>
-      <c r="L16" s="5" t="s">
+      <c r="J17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="6">
+        <v>1</v>
+      </c>
+      <c r="L17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M17" t="s">
         <v>55</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:14">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="3" t="s">
+      <c r="C18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="4">
-        <v>1</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M17" s="3" t="s">
+      <c r="J18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:14">
+      <c r="A19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="5" t="s">
+      <c r="B19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="6">
-        <v>1</v>
-      </c>
-      <c r="L18" s="5" t="s">
+      <c r="J19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="6">
+        <v>1</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M19" t="s">
         <v>55</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N19" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:14">
+      <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="3" t="s">
+      <c r="C20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="4">
-        <v>1</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M19" s="3" t="s">
+      <c r="J20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="N20" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
-      <c r="A20" t="s">
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" t="s">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" t="s">
         <v>16</v>
       </c>
-      <c r="J20" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="2">
+      <c r="J21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="2">
         <v>3</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L21" t="s">
         <v>32</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M21" t="s">
         <v>55</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N21" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="4">
-        <v>1</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="3" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>60</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H22" s="4"/>
       <c r="I22" s="3" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>14</v>
@@ -1573,21 +1574,21 @@
         <v>1</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>98</v>
@@ -1623,86 +1624,86 @@
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" t="s">
+      <c r="D25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" t="s">
         <v>25</v>
       </c>
-      <c r="J24" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="J25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
         <v>32</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M25" t="s">
         <v>55</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N25" s="5" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="4">
-        <v>1</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>75</v>
@@ -1714,15 +1715,15 @@
         <v>60</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H26" s="4" t="s">
         <v>60</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>14</v>
@@ -1730,23 +1731,63 @@
       <c r="K26" s="4">
         <v>1</v>
       </c>
-      <c r="L26" s="3" t="s">
-        <v>32</v>
+      <c r="L26" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="D27" s="4"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="A27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="D28" s="4"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="K28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>